<commit_message>
Code update for Origin Field
</commit_message>
<xml_diff>
--- a/TestData/Loads.xlsx
+++ b/TestData/Loads.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CustomizeGrid" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="73">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -225,13 +225,26 @@
   </si>
   <si>
     <t>0.11</t>
+  </si>
+  <si>
+    <t>Alaska_1006053950</t>
+  </si>
+  <si>
+    <t>Alaska_1006055219</t>
+  </si>
+  <si>
+    <t>Alaska_1006060329</t>
+  </si>
+  <si>
+    <t>Alaska_1006061652</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,11 +598,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="94.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -720,16 +733,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="10" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -964,11 +977,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1139,18 +1152,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="13" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1531,7 +1544,7 @@
         <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
@@ -1552,6 +1565,50 @@
         <v>34</v>
       </c>
       <c r="N9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1570,12 +1627,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New test Cases updated
</commit_message>
<xml_diff>
--- a/TestData/Loads.xlsx
+++ b/TestData/Loads.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="130">
   <si>
     <t>Automation Test ID</t>
   </si>
@@ -336,40 +336,79 @@
     <t>CHN_1222115323</t>
   </si>
   <si>
-    <t>CHN_0101022155</t>
-  </si>
-  <si>
-    <t>CHN_0104041140</t>
-  </si>
-  <si>
-    <t>CHN_0113114059</t>
-  </si>
-  <si>
-    <t>Mexico_0119120548</t>
-  </si>
-  <si>
     <t>CHN_0128022925</t>
   </si>
   <si>
-    <t>Mexico_0129102403</t>
-  </si>
-  <si>
-    <t>CHN_0224121211</t>
-  </si>
-  <si>
     <t>PUN</t>
   </si>
   <si>
-    <t>CHN_0224121827</t>
-  </si>
-  <si>
-    <t>PUN_0224121828</t>
-  </si>
-  <si>
-    <t>CHN_0224123352</t>
-  </si>
-  <si>
-    <t>PUN_0224123353</t>
+    <t>CHN_0407064146</t>
+  </si>
+  <si>
+    <t>PUN_0407064146</t>
+  </si>
+  <si>
+    <t>CHN_0407065609</t>
+  </si>
+  <si>
+    <t>PUN_0407065609</t>
+  </si>
+  <si>
+    <t>CHN_0409112642</t>
+  </si>
+  <si>
+    <t>PUN_0409112643</t>
+  </si>
+  <si>
+    <t>CHN_0409114440</t>
+  </si>
+  <si>
+    <t>PUN_0409114440</t>
+  </si>
+  <si>
+    <t>CHN_0409120743</t>
+  </si>
+  <si>
+    <t>PUN_0409120744</t>
+  </si>
+  <si>
+    <t>Mexico_0412065309</t>
+  </si>
+  <si>
+    <t>PUN_0412065320</t>
+  </si>
+  <si>
+    <t>Mexico_0419023945</t>
+  </si>
+  <si>
+    <t>PUN_0419023946</t>
+  </si>
+  <si>
+    <t>TAB</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>InActivateShippers_TC005</t>
+  </si>
+  <si>
+    <t>Mexico_0426122105</t>
+  </si>
+  <si>
+    <t>ActivateShippers_TC006</t>
+  </si>
+  <si>
+    <t>Mexico_0426123813</t>
+  </si>
+  <si>
+    <t>PUN_0426123814</t>
+  </si>
+  <si>
+    <t>Mexico_0426125455</t>
+  </si>
+  <si>
+    <t>PUN_0426125456</t>
   </si>
 </sst>
 </file>
@@ -414,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -424,6 +463,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,22 +770,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="110.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="7" width="10.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,16 +795,19 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -773,11 +817,14 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -787,11 +834,14 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -801,11 +851,14 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -815,11 +868,14 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -829,11 +885,14 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -843,11 +902,14 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -857,11 +919,14 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -871,11 +936,14 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -885,11 +953,14 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -899,11 +970,14 @@
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -913,11 +987,14 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>78</v>
       </c>
@@ -927,11 +1004,14 @@
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>79</v>
       </c>
@@ -941,11 +1021,14 @@
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>88</v>
       </c>
@@ -956,10 +1039,13 @@
         <v>9</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>95</v>
       </c>
@@ -970,10 +1056,13 @@
         <v>9</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>95</v>
       </c>
@@ -984,6 +1073,43 @@
         <v>9</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -995,15 +1121,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
     <col min="2" max="10" customWidth="true" width="18.28515625" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
@@ -1114,7 +1238,7 @@
         <v>103</v>
       </c>
       <c r="J3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K3" t="s">
         <v>44</v>
@@ -1149,7 +1273,7 @@
         <v>103</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K4" t="s">
         <v>44</v>
@@ -1184,7 +1308,7 @@
         <v>103</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K5" t="s">
         <v>44</v>
@@ -1219,7 +1343,7 @@
         <v>103</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K6" t="s">
         <v>44</v>
@@ -1254,7 +1378,7 @@
         <v>103</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K7" t="s">
         <v>44</v>
@@ -1289,7 +1413,7 @@
         <v>103</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K8" t="s">
         <v>44</v>
@@ -1324,7 +1448,7 @@
         <v>103</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K9" t="s">
         <v>44</v>
@@ -1359,7 +1483,7 @@
         <v>103</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K10" t="s">
         <v>44</v>
@@ -1394,7 +1518,7 @@
         <v>83</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K11" s="5" t="s">
         <v>44</v>
@@ -1429,7 +1553,7 @@
         <v>83</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K12" s="5" t="s">
         <v>44</v>
@@ -1464,7 +1588,7 @@
         <v>103</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>44</v>
@@ -1499,13 +1623,83 @@
         <v>103</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>44</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1894,10 +2088,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,10 +2304,10 @@
         <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>22</v>
+        <v>111</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>22</v>
@@ -2154,10 +2348,10 @@
         <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>22</v>
+        <v>111</v>
+      </c>
+      <c r="H6" t="s">
+        <v>112</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>22</v>
@@ -2198,10 +2392,10 @@
         <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>22</v>
@@ -2242,10 +2436,10 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="H8" t="s">
+        <v>114</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>22</v>
@@ -2286,10 +2480,10 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="H9" t="s">
+        <v>116</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>22</v>
@@ -2330,10 +2524,10 @@
         <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>105</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="H10" t="s">
+        <v>116</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>22</v>
@@ -2373,11 +2567,11 @@
       <c r="F11" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>112</v>
+      <c r="G11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" t="s">
+        <v>108</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>22</v>
@@ -2417,11 +2611,11 @@
       <c r="F12" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>112</v>
+      <c r="G12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" t="s">
+        <v>108</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>22</v>
@@ -2461,11 +2655,11 @@
       <c r="F13" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>112</v>
+      <c r="G13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" t="s">
+        <v>108</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>22</v>
@@ -2506,10 +2700,10 @@
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H14" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>22</v>
@@ -2553,7 +2747,7 @@
         <v>103</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>22</v>
@@ -2597,7 +2791,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>22</v>
@@ -2638,10 +2832,10 @@
         <v>29</v>
       </c>
       <c r="G17" t="s">
-        <v>110</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>22</v>
+        <v>117</v>
+      </c>
+      <c r="H17" t="s">
+        <v>118</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>22</v>
@@ -2682,10 +2876,10 @@
         <v>29</v>
       </c>
       <c r="G18" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>22</v>
+        <v>119</v>
+      </c>
+      <c r="H18" t="s">
+        <v>120</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>22</v>
@@ -2773,7 +2967,7 @@
         <v>103</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>22</v>
@@ -2791,6 +2985,94 @@
         <v>34</v>
       </c>
       <c r="N20" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" t="s">
+        <v>126</v>
+      </c>
+      <c r="H21" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" t="s">
+        <v>129</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="7" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>